<commit_message>
adding tables of analysis for colorado paper
</commit_message>
<xml_diff>
--- a/dataFiles/io/Tables_subregional_Colorado.xlsx
+++ b/dataFiles/io/Tables_subregional_Colorado.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15780" tabRatio="759" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15780" tabRatio="759" firstSheet="3" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="master_table" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Policy" sheetId="11" r:id="rId10"/>
     <sheet name="GCAMdata-ThermalCooling" sheetId="12" r:id="rId11"/>
     <sheet name="GCAMdata-waterperland" sheetId="13" r:id="rId12"/>
+    <sheet name="GCAMdata-animalWaterDemands" sheetId="14" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">demand!$A$1:$K$157</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2908" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2918" uniqueCount="278">
   <si>
     <t>param</t>
   </si>
@@ -972,6 +973,36 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>Coefficient (L/day-animal)</t>
+  </si>
+  <si>
+    <t>Beef cattle</t>
+  </si>
+  <si>
+    <t>Dairy cattle</t>
+  </si>
+  <si>
+    <t>Broiler chicken</t>
+  </si>
+  <si>
+    <t>Layer chicken</t>
+  </si>
+  <si>
+    <t>Pig</t>
+  </si>
+  <si>
+    <t>Sheep</t>
+  </si>
+  <si>
+    <t>Goat</t>
+  </si>
+  <si>
+    <t>Horse</t>
   </si>
 </sst>
 </file>
@@ -1636,7 +1667,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -1761,14 +1792,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1785,6 +1808,17 @@
     </xf>
     <xf numFmtId="2" fontId="18" fillId="36" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2215,8 +2249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K259"/>
   <sheetViews>
-    <sheetView topLeftCell="A223" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B254" sqref="B254"/>
+    <sheetView topLeftCell="A136" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H160" sqref="H160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6795,7 +6829,7 @@
         <v>6.7310672000000003E-5</v>
       </c>
       <c r="H158" s="40">
-        <f t="shared" si="15"/>
+        <f>VLOOKUP(I158,$A$255:$B$256,2,FALSE)*G158</f>
         <v>6.0579604800000002E-5</v>
       </c>
       <c r="I158" s="11" t="s">
@@ -8582,35 +8616,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="32.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="76" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="77" t="s">
         <v>250</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="77" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="78" t="s">
         <v>252</v>
       </c>
-      <c r="B2" s="83">
+      <c r="B2" s="79">
         <v>49.54</v>
       </c>
-      <c r="C2" s="83">
+      <c r="C2" s="79">
         <v>0.38</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="78" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="83">
+      <c r="B3" s="79">
         <v>147.06</v>
       </c>
-      <c r="C3" s="83">
+      <c r="C3" s="79">
         <v>0.91</v>
       </c>
     </row>
@@ -8624,7 +8658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -8638,178 +8672,269 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="81" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="81" t="s">
         <v>264</v>
       </c>
-      <c r="C1" s="85" t="s">
+      <c r="C1" s="81" t="s">
         <v>266</v>
       </c>
-      <c r="D1" s="85" t="s">
+      <c r="D1" s="81" t="s">
         <v>265</v>
       </c>
-      <c r="E1" s="85" t="s">
+      <c r="E1" s="81" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="80" t="s">
         <v>254</v>
       </c>
-      <c r="B2" s="84">
-        <v>2010</v>
-      </c>
-      <c r="C2" s="86">
+      <c r="B2" s="80">
+        <v>2010</v>
+      </c>
+      <c r="C2" s="82">
         <v>4.2483529999999999E-2</v>
       </c>
-      <c r="D2" s="86">
+      <c r="D2" s="82">
         <v>4.9053180000000002E-2</v>
       </c>
-      <c r="E2" s="86">
+      <c r="E2" s="82">
         <v>0.86607089999999998</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="80" t="s">
         <v>255</v>
       </c>
-      <c r="B3" s="84">
-        <v>2010</v>
-      </c>
-      <c r="C3" s="86">
+      <c r="B3" s="80">
+        <v>2010</v>
+      </c>
+      <c r="C3" s="82">
         <v>4.200707E-4</v>
       </c>
-      <c r="D3" s="86">
+      <c r="D3" s="82">
         <v>6.9139799999999997E-4</v>
       </c>
-      <c r="E3" s="86">
+      <c r="E3" s="82">
         <v>0.60756719999999997</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="84" t="s">
+      <c r="A4" s="80" t="s">
         <v>256</v>
       </c>
-      <c r="B4" s="84">
-        <v>2010</v>
-      </c>
-      <c r="C4" s="86">
+      <c r="B4" s="80">
+        <v>2010</v>
+      </c>
+      <c r="C4" s="82">
         <v>0.13459199999999999</v>
       </c>
-      <c r="D4" s="86">
+      <c r="D4" s="82">
         <v>0.24686859999999999</v>
       </c>
-      <c r="E4" s="86">
+      <c r="E4" s="82">
         <v>0.54519689999999998</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="80" t="s">
         <v>257</v>
       </c>
-      <c r="B5" s="84">
-        <v>2010</v>
-      </c>
-      <c r="C5" s="86">
+      <c r="B5" s="80">
+        <v>2010</v>
+      </c>
+      <c r="C5" s="82">
         <v>1.60221904</v>
       </c>
-      <c r="D5" s="86">
+      <c r="D5" s="82">
         <v>4.6400347999999996</v>
       </c>
-      <c r="E5" s="86">
+      <c r="E5" s="82">
         <v>0.34530319999999998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="84" t="s">
+      <c r="A6" s="80" t="s">
         <v>258</v>
       </c>
-      <c r="B6" s="84">
-        <v>2010</v>
-      </c>
-      <c r="C6" s="86">
+      <c r="B6" s="80">
+        <v>2010</v>
+      </c>
+      <c r="C6" s="82">
         <v>0.13348789999999999</v>
       </c>
-      <c r="D6" s="86">
+      <c r="D6" s="82">
         <v>9.3928600000000001E-2</v>
       </c>
-      <c r="E6" s="86">
+      <c r="E6" s="82">
         <v>1.4211635</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="80" t="s">
         <v>259</v>
       </c>
-      <c r="B7" s="84">
-        <v>2010</v>
-      </c>
-      <c r="C7" s="86">
+      <c r="B7" s="80">
+        <v>2010</v>
+      </c>
+      <c r="C7" s="82">
         <v>3.0225229999999999E-2</v>
       </c>
-      <c r="D7" s="86">
+      <c r="D7" s="82">
         <v>0.1095454</v>
       </c>
-      <c r="E7" s="86">
+      <c r="E7" s="82">
         <v>0.27591510000000002</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="84" t="s">
+      <c r="A8" s="80" t="s">
         <v>260</v>
       </c>
-      <c r="B8" s="84">
-        <v>2010</v>
-      </c>
-      <c r="C8" s="86">
+      <c r="B8" s="80">
+        <v>2010</v>
+      </c>
+      <c r="C8" s="82">
         <v>1.322075E-4</v>
       </c>
-      <c r="D8" s="86">
+      <c r="D8" s="82">
         <v>2.33E-4</v>
       </c>
-      <c r="E8" s="86">
+      <c r="E8" s="82">
         <v>0.56741419999999998</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="80" t="s">
         <v>261</v>
       </c>
-      <c r="B9" s="84">
-        <v>2010</v>
-      </c>
-      <c r="C9" s="86">
+      <c r="B9" s="80">
+        <v>2010</v>
+      </c>
+      <c r="C9" s="82">
         <v>5.6669490000000003E-2</v>
       </c>
-      <c r="D9" s="86">
+      <c r="D9" s="82">
         <v>0.14153018000000001</v>
       </c>
-      <c r="E9" s="86">
+      <c r="E9" s="82">
         <v>0.40040569999999998</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="84" t="s">
+      <c r="A10" s="80" t="s">
         <v>262</v>
       </c>
-      <c r="B10" s="84">
-        <v>2010</v>
-      </c>
-      <c r="C10" s="86">
+      <c r="B10" s="80">
+        <v>2010</v>
+      </c>
+      <c r="C10" s="82">
         <v>0.10841133</v>
       </c>
-      <c r="D10" s="86">
+      <c r="D10" s="82">
         <v>0.15162538</v>
       </c>
-      <c r="E10" s="86">
+      <c r="E10" s="82">
         <v>0.71499460000000004</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="A1:B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="87" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="79" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="79">
+        <v>34.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="79" t="s">
+        <v>271</v>
+      </c>
+      <c r="B3" s="79">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="79" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" s="79">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="79" t="s">
+        <v>273</v>
+      </c>
+      <c r="B5" s="79">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="79" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="79">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="79" t="s">
+        <v>275</v>
+      </c>
+      <c r="B7" s="79">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="79" t="s">
+        <v>276</v>
+      </c>
+      <c r="B8" s="79">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="79" t="s">
+        <v>277</v>
+      </c>
+      <c r="B9" s="79">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -8817,8 +8942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K164"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14046,18 +14171,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I1" s="76" t="s">
+      <c r="I1" s="83" t="s">
         <v>141</v>
       </c>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="78" t="s">
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" s="74" t="s">
@@ -16625,7 +16750,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>